<commit_message>
Changed taint table for MULT
</commit_message>
<xml_diff>
--- a/hw5/taint_tables.xlsx
+++ b/hw5/taint_tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>e</t>
   </si>
@@ -35,12 +35,21 @@
   <si>
     <t>Table 3. Taint inheritance for || expression.</t>
   </si>
+  <si>
+    <t>Table 4. Taint inheritance for * expression.</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>!0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +80,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -151,15 +166,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -173,6 +191,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -476,46 +506,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:F15"/>
+      <selection activeCell="A17" sqref="A17:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="b">
+      <c r="D3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="b">
@@ -523,7 +553,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="b">
@@ -543,8 +573,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="b">
+      <c r="A5" s="6"/>
+      <c r="B5" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="b">
@@ -561,8 +591,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="b">
+      <c r="A6" s="6"/>
+      <c r="B6" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="b">
@@ -579,7 +609,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="3" t="b">
         <v>1</v>
       </c>
@@ -597,37 +627,37 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="D11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5" t="b">
+      <c r="D11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F11" s="3" t="b">
@@ -635,7 +665,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="3" t="b">
@@ -655,8 +685,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="b">
+      <c r="A13" s="6"/>
+      <c r="B13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C13" s="2" t="b">
@@ -673,8 +703,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="b">
+      <c r="A14" s="6"/>
+      <c r="B14" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
@@ -691,7 +721,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="3" t="b">
         <v>1</v>
       </c>
@@ -708,16 +738,132 @@
         <v>1</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="12">
+        <v>0</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="12">
+        <v>0</v>
+      </c>
+      <c r="C20" s="15">
+        <v>0</v>
+      </c>
+      <c r="D20" s="15">
+        <v>0</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="13">
+        <v>0</v>
+      </c>
+      <c r="C21" s="15">
+        <v>0</v>
+      </c>
+      <c r="D21" s="14">
+        <v>0</v>
+      </c>
+      <c r="E21" s="14">
+        <v>0</v>
+      </c>
+      <c r="F21" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="15">
+        <v>0</v>
+      </c>
+      <c r="D22" s="14">
+        <v>0</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="14">
+        <v>0</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:F18"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="A10:B11"/>
     <mergeCell ref="C10:F10"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>